<commit_message>
Added test points to component PCB; Added 3D mockups
</commit_message>
<xml_diff>
--- a/Measured response of AS3364 VCA control curve.xlsx
+++ b/Measured response of AS3364 VCA control curve.xlsx
@@ -8,16 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eurorack\Ampelope\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2550B0B5-B42E-4EA3-930C-6691B82A1903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291C9B18-AC59-402D-BC80-DA83FB192669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8856" yWindow="132" windowWidth="20904" windowHeight="16680" xr2:uid="{DCF98C69-3E39-45F8-9405-1489E49FA1EB}"/>
+    <workbookView xWindow="9000" yWindow="132" windowWidth="20760" windowHeight="16080" xr2:uid="{DCF98C69-3E39-45F8-9405-1489E49FA1EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$2:$B$10</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$10</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$2:$B$10</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$2:$A$10</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$2:$B$10</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$2:$A$10</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$2:$B$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1327,7 +1334,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="A16:B16"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>